<commit_message>
Added OCR register scan
</commit_message>
<xml_diff>
--- a/Trainee Roster..xlsx
+++ b/Trainee Roster..xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t xml:space="preserve">Trainee ID </t>
   </si>
@@ -161,17 +161,114 @@
   </si>
   <si>
     <t xml:space="preserve">snemshibe5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sbonelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbonelo4@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ziyanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mbonambi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ziyandambonambi@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khanyile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msiro@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sibiya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shante@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melokuhle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melokuhle@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grealish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jack99@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRB07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sbza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">joness2@gmail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.com</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,6 +302,18 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -256,7 +365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,6 +387,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,10 +525,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -457,8 +578,7 @@
       <c r="F2" s="5" t="n">
         <v>37654</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <f aca="true">DATEDIF(F2, TODAY(), "Y")</f>
+      <c r="G2" s="1" t="n">
         <v>22</v>
       </c>
     </row>
@@ -481,9 +601,8 @@
       <c r="F3" s="5" t="n">
         <v>37508</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <f aca="true">DATEDIF(F3, TODAY(), "Y")</f>
-        <v>22</v>
+      <c r="G3" s="1" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,9 +624,8 @@
       <c r="F4" s="5" t="n">
         <v>37320</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <f aca="true">DATEDIF(F4, TODAY(), "Y")</f>
-        <v>23</v>
+      <c r="G4" s="1" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,9 +647,8 @@
       <c r="F5" s="5" t="n">
         <v>37139</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <f aca="true">DATEDIF(F5, TODAY(), "Y")</f>
-        <v>23</v>
+      <c r="G5" s="1" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,8 +670,7 @@
       <c r="F6" s="5" t="n">
         <v>36284</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <f aca="true">DATEDIF(F6, TODAY(), "Y")</f>
+      <c r="G6" s="1" t="n">
         <v>26</v>
       </c>
     </row>
@@ -577,9 +693,8 @@
       <c r="F7" s="5" t="n">
         <v>36842</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <f aca="true">DATEDIF(F7, TODAY(), "Y")</f>
-        <v>24</v>
+      <c r="G7" s="1" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,9 +716,8 @@
       <c r="F8" s="5" t="n">
         <v>38729</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <f aca="true">DATEDIF(F8, TODAY(), "Y")</f>
-        <v>19</v>
+      <c r="G8" s="1" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,9 +739,8 @@
       <c r="F9" s="5" t="n">
         <v>37248</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <f aca="true">DATEDIF(F9, TODAY(), "Y")</f>
-        <v>23</v>
+      <c r="G9" s="1" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,9 +762,8 @@
       <c r="F10" s="5" t="n">
         <v>38565</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <f aca="true">DATEDIF(F10, TODAY(), "Y")</f>
-        <v>19</v>
+      <c r="G10" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,6 +788,179 @@
       <c r="G11" s="0" t="n">
         <f aca="true">DATEDIF(F11, TODAY(), "Y")</f>
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>606218075</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>37553</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="true">DATEDIF(F12, TODAY(), "Y")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>761967291</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>37990</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="true">DATEDIF(F13, TODAY(), "Y")</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>831234567</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>38427</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="true">DATEDIF(F14, TODAY(), "Y")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>638798411</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>40248</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="true">DATEDIF(F15, TODAY(), "Y")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>827382793</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>36904</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="true">DATEDIF(F16, TODAY(), "Y")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>728634291</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>35169</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="true">DATEDIF(F17, TODAY(), "Y")</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>658328108</v>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>34130</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="true">DATEDIF(F18, TODAY(), "Y")</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D19" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -690,6 +975,13 @@
     <hyperlink ref="D9" r:id="rId8" display="mpume90@gmail.com"/>
     <hyperlink ref="D10" r:id="rId9" display="lungelomthembu@gmail.com"/>
     <hyperlink ref="D11" r:id="rId10" display="snemshibe5@gmail.com"/>
+    <hyperlink ref="D12" r:id="rId11" display="cbonelo4@gmail.com"/>
+    <hyperlink ref="D13" r:id="rId12" display="ziyandambonambi@gmail.com"/>
+    <hyperlink ref="D14" r:id="rId13" display="msiro@gmail.com"/>
+    <hyperlink ref="D15" r:id="rId14" display="shante@gmail.com"/>
+    <hyperlink ref="D16" r:id="rId15" display="melokuhle@gmail.com"/>
+    <hyperlink ref="D17" r:id="rId16" display="jack99@gmail.com"/>
+    <hyperlink ref="D18" r:id="rId17" display="joness2@gmail"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>